<commit_message>
Added assertions and logged it to the report for user API.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/user_testdata.xlsx
+++ b/src/test/resources/excel/user_testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\git\BDDRestAssuredUserAPITeamBJan22\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\git\NinjaCoderLMSRestAssured\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF6AC38-7E8D-49F9-892C-233A25E4F15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8898D7E4-41E4-4E68-AAA3-378D9F8E7B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
   <si>
     <t>Test case Name</t>
   </si>
@@ -463,10 +463,7 @@
 }</t>
   </si>
   <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>U297</t>
+    <t>U393</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1401,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1431,10 +1428,10 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Updated log4j files and added delete db validation for Skills API
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/user_testdata.xlsx
+++ b/src/test/resources/excel/user_testdata.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\git\NinjaCoderLMSRestAssured\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8898D7E4-41E4-4E68-AAA3-378D9F8E7B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="get" sheetId="4" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="put" sheetId="2" r:id="rId3"/>
     <sheet name="delete" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -469,8 +463,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -571,9 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -636,7 +627,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -671,7 +662,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -850,22 +841,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -882,7 +873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -899,7 +890,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -916,7 +907,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -930,7 +921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -947,7 +938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -964,7 +955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -981,7 +972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -998,7 +989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1015,7 +1006,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1031,13 +1022,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C7" r:id="rId4"/>
+    <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId8"/>
@@ -1045,22 +1036,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="60.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5546875" customWidth="1"/>
+    <col min="1" max="1" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5703125" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="165">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1088,7 +1079,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="135">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1102,7 +1093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="165">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1116,7 +1107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="165">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1130,7 +1121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="165">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1144,7 +1135,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="165">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1158,7 +1149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="165">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1172,7 +1163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="165">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1186,7 +1177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="165">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1200,7 +1191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="165">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1221,23 +1212,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="44.109375" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1254,14 +1245,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="225">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -1271,7 +1262,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="225">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1279,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="225">
       <c r="A4" s="11" t="s">
         <v>20</v>
       </c>
@@ -1305,7 +1296,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="210">
       <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
@@ -1322,7 +1313,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="210">
       <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
@@ -1339,7 +1330,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="210">
       <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
@@ -1356,7 +1347,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="225">
       <c r="A8" s="11" t="s">
         <v>24</v>
       </c>
@@ -1373,7 +1364,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="240">
       <c r="A9" s="11" t="s">
         <v>25</v>
       </c>
@@ -1397,19 +1388,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="31" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1423,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -1437,7 +1428,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
@@ -1451,7 +1442,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1465,55 +1456,55 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="6"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>

</xml_diff>

<commit_message>
Updated Log4j for Skills and UserSkill api and updated pom
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/user_testdata.xlsx
+++ b/src/test/resources/excel/user_testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="get" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
   <si>
     <t>Test case Name</t>
   </si>
@@ -109,15 +109,9 @@
     <t>To delete the user with invalid user id</t>
   </si>
   <si>
-    <t>U12</t>
-  </si>
-  <si>
     <t>U17</t>
   </si>
   <si>
-    <t>U23</t>
-  </si>
-  <si>
     <t>U72</t>
   </si>
   <si>
@@ -187,174 +181,10 @@
     <t>To check if able to read record with userId as decimal</t>
   </si>
   <si>
-    <t>{
-"name": "Rita,Dcruz",
-"phone_number": 4298490488,
-"location": "seattle",
-"time_zone": "EST",
-"linkedin_url": "https://www.linkedin.com/in/Rita Dcruz/",
-"education_ug": "Computer Science Engineering",
-"education_pg": " MBA",
-"visa_status": "Not-Specified",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
     <t>User successfully Created!</t>
   </si>
   <si>
-    <t>{
-"name": "Myra,",
-"phone_number": 123466890,
-"location": "New York",
-"time_zone": "PST",
-"linkedin_url": "https://www.linkedin.com/in/Myra/",
-"education_ug": "Computer Science Engineering",
-"education_pg": "MBA",
-"visa_status": "Not-Specified",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
     <t>To create user record with visa status and location blank</t>
-  </si>
-  <si>
-    <t>{
-"name": ",Pinto",
-"phone_number": 1234557890,
-"location": "Cannada",
-"time_zone": "PST",
-"linkedin_url": "https://www.linkedin.com/in/Pinto/",
-"education_ug": "Computer Science Engineering",
-"education_pg": "MBA",
-"visa_status": "Not-Specified",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>{
-"name": "123ADFG,Smith",
-"phone_number": 1234557890,
-"location": "Ne763ork",
-"time_zone": "PST",
-"linkedin_url": "https://www.linkedin.com/in/123ADFG Smith/",
-"education_ug": "Electronics Engineering",
-"education_pg": "BTech",
-"visa_status": "H4-EAD",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>{
-"name": "Sam,Tucker",
-"phone_number": 2912345678,
-"location": "India",
-"time_zone": "IST",
-"linkedin_url": "12SFGH@linkedin#%$%^",
-"education_ug": "Computer Science",
-"education_pg": "",
-"visa_status": "H4-EAD",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>{
-"name": "Rachel,Hansen",
-"phone_number": 9087629128,
-"location": "USA",
-"time_zone": "OOO",
-"linkedin_url": "https://www.linkedin.com/in/Rachel Hansen/",
-"education_ug": "Computer Science",
-"education_pg": "MS",
-"visa_status": "H1B",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-"name": "Elisha,Hope",
-"phone_number": 9753281287,
-"location": "Michigan",
-"time_zone": "EST",
-"linkedin_url": "",
-"education_ug": "Computer Science",
-"education_pg": "",
-"visa_status": "Not-Specified",
-"comments": ""
-} </t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U12",
-    "name": "Sarah,Zack",
-    "phone_number": 9057654321,
-    "location": "Canada",
-    "time_zone": "EST",
-    "linkedin_url": "https://www.linkedin.com/in/Sarah Zack/",
-    "education_ug": "Computer Science Engineering",
-    "education_pg": "MS",
-    "visa_status": "H1B",
-    "comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U12",
-    "name": "Sarah,67493Zack",
-    "phone_number": 9057654321,
-    "location": "Canada123",
-    "time_zone": "EST",
-    "linkedin_url": "https://www.linkedin.com/in/Sarah Zack/",
-    "education_ug": "Computer Science Engineering",
-    "education_pg": "MS",
-    "visa_status": "H1B",
-    "comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U23",
-    "name": "Zeek,Roy",
-    "phone_number": 1234667890,
-    "location": "New 12345",
-    "time_zone": "CST",
-    "linkedin_url": "https://www.linkedin.com/in/Zeek Roy/",
-    "education_ug": "Robotics",
-    "education_pg": "MS",
-    "visa_status": "US-Citizen",
-    "comments": "Tes4592759t"
-}</t>
-  </si>
-  <si>
-    <t>U48</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U48",
-    "name": "Preeti,Gupta",
-    "phone_number": 1234667890,
-    "location": "New York",
-    "time_zone": "CST",
-    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
-    "education_ug": "BTech",
-    "education_pg": "MTech",
-    "visa_status": "Not-Specified",
-    "comments": "Test"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U48",
-    "name": "Preeti,Gupta",
-    "phone_number": 1234667890,
-    "location": "New York",
-    "time_zone": "ZST",
-    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
-    "education_ug": "BTech",
-    "education_pg": "MTech",
-    "visa_status": "Not-Specified",
-    "comments": "Tes4592759t"
-}</t>
   </si>
   <si>
     <t>{
@@ -406,30 +236,6 @@
     <t>To check if able to read record with userId as blank</t>
   </si>
   <si>
-    <t>{
-"name": "Megha,Patel",
-"phone_number": 9123456788,
-"time_zone": "EST",
-"linkedin_url": "https://www.linkedin.com/in/Patel/",
-"education_ug": "Electronic Engineering",
-"education_pg": "MBA",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>{
-"name": "Newton,Krill",
-"phone_number": "lkjhgfdsaw",
-"location": "Texas",
-"time_zone": "EST",
-"linkedin_url": "https://www.linkedin.com/in/Newton Krill/",
-"education_ug": "Computer Science",
-"education_pg": "MS",
-"visa_status": "Not-Specified",
-"comments": "Test"
-}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{
 "name": "Zack,Reader",
 "phone_number": 9753281287,
@@ -444,7 +250,129 @@
   </si>
   <si>
     <t>{
-    "user_id": "U17",
+"name": "Shilpa,Patel",
+"phone_number": 9120006788,
+"time_zone": "EST",
+"linkedin_url": "https://www.linkedin.com/in/Patel/",
+"education_ug": "Electronic Engineering",
+"education_pg": "MBA",
+"comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>{
+"name": ",Zinta",
+"phone_number": 1234557890,
+"location": "Cannada",
+"time_zone": "PST",
+"linkedin_url": "https://www.linkedin.com/in/Zinta/",
+"education_ug": "Computer Science Engineering",
+"education_pg": "MBA",
+"visa_status": "Not-Specified",
+"comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>{
+"name": "Siara,",
+"phone_number": 123466890,
+"location": "New York",
+"time_zone": "PST",
+"linkedin_url": "https://www.linkedin.com/in/Siara/",
+"education_ug": "Computer Science Engineering",
+"education_pg": "MBA",
+"visa_status": "Not-Specified",
+"comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>{
+"name": "Ruchi,Dcruz",
+"phone_number": 4298490488,
+"location": "seattle",
+"time_zone": "EST",
+"linkedin_url": "https://www.linkedin.com/in/Ruchi Dcruz/",
+"education_ug": "Computer Science Engineering",
+"education_pg": " MBA",
+"visa_status": "Not-Specified",
+"comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>{
+"name": "Sam,Dunkan",
+"phone_number": 2912345678,
+"location": "India",
+"time_zone": "IST",
+"linkedin_url": "12SFGH@linkedin#%$%^",
+"education_ug": "Computer Science",
+"education_pg": "",
+"visa_status": "H4-EAD",
+"comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>{
+"name": "Harry,Hansen",
+"phone_number": 9087629128,
+"location": "USA",
+"time_zone": "AA",
+"linkedin_url": "https://www.linkedin.com/in/Harry Hansen/",
+"education_ug": "Computer Science",
+"education_pg": "MS",
+"visa_status": "H1B",
+"comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+"name": "Swathi,Hope",
+"phone_number": 9753281287,
+"location": "Michigan",
+"time_zone": "EST",
+"linkedin_url": "",
+"education_ug": "Computer Science",
+"education_pg": "",
+"visa_status": "Not-Specified",
+"comments": ""
+} </t>
+  </si>
+  <si>
+    <t>{
+"name": "Newton,Krill",
+"phone_number": "aaabbbccc",
+"location": "Texas",
+"time_zone": "EST",
+"linkedin_url": "https://www.linkedin.com/in/Newton Krill/",
+"education_ug": "Computer Science",
+"education_pg": "MS",
+"visa_status": "Not-Specified",
+"comments": "Test"
+}</t>
+  </si>
+  <si>
+    <t>U08</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U08",
+    "name": "Sarah,Travis",
+    "phone_number": 9057654321,
+    "location": "Canada",
+    "time_zone": "EST",
+    "linkedin_url": "https://www.linkedin.com/in/Sarah Zack/",
+    "education_ug": "Computer Science Engineering",
+    "education_pg": "MS",
+    "visa_status": "H1B",
+    "comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>U27</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U27",
     "name": "Sam,Axe",
     "phone_number": "9876slrm321",
     "location": "Arizona",
@@ -457,7 +385,82 @@
 }</t>
   </si>
   <si>
-    <t>U393</t>
+    <t>{
+    "user_id": "U08",
+    "name": "Sarah,674777ack",
+    "phone_number": 9057654321,
+    "location": "Canada123",
+    "time_zone": "EST",
+    "linkedin_url": "https://www.linkedin.com/in/Sarah Zack/",
+    "education_ug": "Computer Science Engineering",
+    "education_pg": "MS",
+    "visa_status": "H1B",
+    "comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>U115</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U115",
+    "name": "Ellisha,hope",
+    "phone_number": 1234667890,
+    "location": "New York",
+    "time_zone": "CST",
+    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
+    "education_ug": "BTech",
+    "education_pg": "MTech",
+    "visa_status": "Not-Specified",
+    "comments": "Test"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U17",
+    "name": "Zeek,Roy",
+    "phone_number": 1234667890,
+    "location": "New 12345",
+    "time_zone": "CST",
+    "linkedin_url": "https://www.linkedin.com/in/Zeek Roy/",
+    "education_ug": "Robotics",
+    "education_pg": "MS",
+    "visa_status": "US-Citizen",
+    "comments": "Tes4592759t"
+}</t>
+  </si>
+  <si>
+    <t>U40</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U40",
+    "name": "Shinoj,Accart",
+    "phone_number": 1234667890,
+    "location": "New York",
+    "time_zone": "ZST",
+    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
+    "education_ug": "BTech",
+    "education_pg": "MTech",
+    "visa_status": "Not-Specified",
+    "comments": "Tes4592759t"
+}</t>
+  </si>
+  <si>
+    <t>U124</t>
+  </si>
+  <si>
+    <t>{
+"name": "200ADF,John",
+"phone_number": 12345521430,
+"location": "Ne763ork",
+"time_zone": "PST",
+"linkedin_url": "https://www.linkedin.com/in/123ADFG John/",
+"education_ug": "Electronics Engineering",
+"education_pg": "BTech",
+"visa_status": "H4-EAD",
+"comments": "Hello"
+}</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -565,6 +568,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -845,15 +854,15 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -861,10 +870,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>17</v>
@@ -875,47 +884,47 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>10</v>
@@ -923,16 +932,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>10</v>
@@ -940,16 +949,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>14</v>
@@ -957,16 +966,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>14</v>
@@ -974,16 +983,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>14</v>
@@ -991,16 +1000,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>14</v>
@@ -1008,13 +1017,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>10</v>
@@ -1039,16 +1048,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5703125" customWidth="1"/>
+    <col min="1" max="1" width="60.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.54296875" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1065,26 +1074,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="165">
+    <row r="2" spans="1:4" ht="159.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="135">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="130.5">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -1093,12 +1102,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="165">
+    <row r="4" spans="1:4" ht="159.5">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -1107,12 +1116,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="165">
+    <row r="5" spans="1:4" ht="159.5">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -1121,26 +1130,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="165">
+    <row r="6" spans="1:4" ht="159.5">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="165">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="159.5">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -1149,12 +1158,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="165">
+    <row r="8" spans="1:4" ht="159.5">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
@@ -1163,12 +1172,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="165">
+    <row r="9" spans="1:4" ht="159.5">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
@@ -1177,12 +1186,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="165">
+    <row r="10" spans="1:4" ht="159.5">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
@@ -1191,18 +1200,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="165">
+    <row r="11" spans="1:4" ht="159.5">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1215,17 +1224,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="35.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" customWidth="1"/>
+    <col min="5" max="5" width="44.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1245,49 +1254,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="225">
+    <row r="2" spans="1:5" ht="217.5">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>30</v>
+      <c r="B2" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="225">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="217.5">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>66</v>
+      <c r="B3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>78</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="225">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="217.5">
       <c r="A4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>83</v>
+      <c r="B4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>77</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>14</v>
@@ -1296,49 +1305,49 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="210">
+    <row r="5" spans="1:5" ht="203">
       <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>67</v>
+      <c r="B5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="210">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="203">
       <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>69</v>
+      <c r="B6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="210">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="203">
       <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>70</v>
+      <c r="B7" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>14</v>
@@ -1347,32 +1356,32 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="225">
+    <row r="8" spans="1:5" ht="217.5">
       <c r="A8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="240">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="232">
       <c r="A9" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>14</v>
@@ -1392,12 +1401,12 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="31" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1425,15 +1434,15 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>27</v>
@@ -1447,7 +1456,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
updated code removed testng dependency
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/user_testdata.xlsx
+++ b/src/test/resources/excel/user_testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12720" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="28610" windowHeight="15160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="get" sheetId="4" r:id="rId1"/>
@@ -236,19 +236,6 @@
     <t>To check if able to read record with userId as blank</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-"name": "Zack,Reader",
-"phone_number": 9753281287,
-"location": "Toronto",
-"time_zone": "CST",
-"linkedin_url": "https://www.linkedin.com/in/Zack Reader/",
-"education_ug": "Computer Science",
-"education_pg": "MS",
-"visa_status": 1234,
-"comments": "Hello"
-}  </t>
-  </si>
-  <si>
     <t>{
 "name": "Shilpa,Patel",
 "phone_number": 9120006788,
@@ -461,6 +448,19 @@
 "visa_status": "H4-EAD",
 "comments": "Hello"
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+"name": "Zack,Reader",
+"phone_number": 9753281287,
+"location": "Toronto",
+"time_zone": "CST",
+"linkedin_url": "https://www.linkedin.com/in/Zack Reader/",
+"education_ug": "Computer Science",
+"education_pg": "MS",
+"visa_status": 4521,
+"comments": "Hello"
+}  </t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1079,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
@@ -1093,7 +1093,7 @@
         <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -1107,7 +1107,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -1121,7 +1121,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -1135,7 +1135,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
@@ -1149,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -1163,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
@@ -1177,7 +1177,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
@@ -1191,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
@@ -1205,7 +1205,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
@@ -1259,10 +1259,10 @@
         <v>16</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>10</v>
@@ -1276,10 +1276,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>10</v>
@@ -1293,10 +1293,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>76</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>77</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>14</v>
@@ -1313,7 +1313,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>10</v>
@@ -1327,10 +1327,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>79</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>80</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>10</v>
@@ -1344,10 +1344,10 @@
         <v>23</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>14</v>
@@ -1428,7 +1428,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Code clean and test data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/user_testdata.xlsx
+++ b/src/test/resources/excel/user_testdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a27db815e8f35ce/Desktop/API Hackathon/LatestCode/NinjaCoderLMSRestAssured latest/NinjaCoderLMSRestAssured/src/test/resources/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:801_{B3352A4E-2F49-49F2-92EA-8DBA3CFDA0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1521E94-14A5-416A-86AE-A5D23797E78F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="28610" windowHeight="15160" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get" sheetId="4" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="put" sheetId="2" r:id="rId3"/>
     <sheet name="delete" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="90">
   <si>
     <t>Test case Name</t>
   </si>
@@ -43,9 +49,6 @@
     <t>Body</t>
   </si>
   <si>
-    <t>To create User Record with blank linkedin_url, education_pg, comments</t>
-  </si>
-  <si>
     <t>StatusCode</t>
   </si>
   <si>
@@ -107,9 +110,6 @@
   </si>
   <si>
     <t>To delete the user with invalid user id</t>
-  </si>
-  <si>
-    <t>U17</t>
   </si>
   <si>
     <t>U72</t>
@@ -338,105 +338,6 @@
 }</t>
   </si>
   <si>
-    <t>U08</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U08",
-    "name": "Sarah,Travis",
-    "phone_number": 9057654321,
-    "location": "Canada",
-    "time_zone": "EST",
-    "linkedin_url": "https://www.linkedin.com/in/Sarah Zack/",
-    "education_ug": "Computer Science Engineering",
-    "education_pg": "MS",
-    "visa_status": "H1B",
-    "comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>U27</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U27",
-    "name": "Sam,Axe",
-    "phone_number": "9876slrm321",
-    "location": "Arizona",
-    "time_zone": "EST",
-    "linkedin_url": "https://www.linkedin.com/in/Sam Axe/",
-    "education_ug": "Computer Science Engineering",
-    "education_pg": "MS",
-    "visa_status": "US-Citizen",
-    "comments": "Test"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U08",
-    "name": "Sarah,674777ack",
-    "phone_number": 9057654321,
-    "location": "Canada123",
-    "time_zone": "EST",
-    "linkedin_url": "https://www.linkedin.com/in/Sarah Zack/",
-    "education_ug": "Computer Science Engineering",
-    "education_pg": "MS",
-    "visa_status": "H1B",
-    "comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>U115</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U115",
-    "name": "Ellisha,hope",
-    "phone_number": 1234667890,
-    "location": "New York",
-    "time_zone": "CST",
-    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
-    "education_ug": "BTech",
-    "education_pg": "MTech",
-    "visa_status": "Not-Specified",
-    "comments": "Test"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U17",
-    "name": "Zeek,Roy",
-    "phone_number": 1234667890,
-    "location": "New 12345",
-    "time_zone": "CST",
-    "linkedin_url": "https://www.linkedin.com/in/Zeek Roy/",
-    "education_ug": "Robotics",
-    "education_pg": "MS",
-    "visa_status": "US-Citizen",
-    "comments": "Tes4592759t"
-}</t>
-  </si>
-  <si>
-    <t>U40</t>
-  </si>
-  <si>
-    <t>{
-    "user_id": "U40",
-    "name": "Shinoj,Accart",
-    "phone_number": 1234667890,
-    "location": "New York",
-    "time_zone": "ZST",
-    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
-    "education_ug": "BTech",
-    "education_pg": "MTech",
-    "visa_status": "Not-Specified",
-    "comments": "Tes4592759t"
-}</t>
-  </si>
-  <si>
-    <t>U124</t>
-  </si>
-  <si>
     <t>{
 "name": "200ADF,John",
 "phone_number": 12345521430,
@@ -462,12 +363,139 @@
 "comments": "Hello"
 }  </t>
   </si>
+  <si>
+    <t>To create User with duplicate record</t>
+  </si>
+  <si>
+    <t>To create User record with blank linkedin_url, education_pg, comments</t>
+  </si>
+  <si>
+    <t>To create record with phone number less than ten digits</t>
+  </si>
+  <si>
+    <t>{
+"name": "Mark,Reeves",
+"phone_number": 93281,
+"location": "Waxhaw",
+"time_zone": "EST",
+"linkedin_url": "https://www.linkedin.com/in/Mark Reeves/",
+"education_ug": "Computer Science",
+"education_pg": "MS",
+"visa_status": "Not-Specified",
+"comments": "Citizen"
+}</t>
+  </si>
+  <si>
+    <t>To Check Authorization with valid username and password</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U03",
+    "name": "Mary,Poppins",
+    "phone_number": 9057654321,
+    "location": "Canada",
+    "time_zone": "EST",
+    "linkedin_url": "https://www.linkedin.com/in/Sarah Zack/",
+    "education_ug": "Computer Science Engineering",
+    "education_pg": "MS",
+    "visa_status": "H1B",
+    "comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>U06</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U06",
+    "name": "Sylvia,674777ack",
+    "phone_number": 9562009911,
+    "location": "India123",
+    "time_zone": "IST",
+    "linkedin_url": "https://www.linkedin.com/in/Sylvia674777ack/",
+    "education_ug": "Computer Science Engineering",
+    "education_pg": "MS",
+    "visa_status": "H1B",
+    "comments": "Hello"
+}</t>
+  </si>
+  <si>
+    <t>U143</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U143",
+    "name": "Sam,Axe",
+    "phone_number": "9876slrm321",
+    "location": "Arizona",
+    "time_zone": "EST",
+    "linkedin_url": "https://www.linkedin.com/in/Sam Axe/",
+    "education_ug": "Electronics and Electrical Engineering",
+    "education_pg": " Computer Technology",
+    "visa_status": "H4-EAD",
+    "comments": "Test"
+}</t>
+  </si>
+  <si>
+    <t>U148</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U148",
+    "name": "Zeek,Roy",
+    "phone_number": 1234667890,
+    "location": "New 12345",
+    "time_zone": "CST",
+    "linkedin_url": "https://www.linkedin.com/in/Zeek Roy/",
+    "education_ug": "Robotics",
+    "education_pg": "MS",
+    "visa_status": "US-Citizen",
+    "comments": "Tes4592759t"
+}</t>
+  </si>
+  <si>
+    <t>U112</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U112",
+    "name": "Ellisha,hope",
+    "phone_number": 1234667890,
+    "location": "New York",
+    "time_zone": "CST",
+    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
+    "education_ug": "BTech",
+    "education_pg": "MTech",
+    "visa_status": "Not-Specified",
+    "comments": "Test"
+}</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>{
+    "user_id": "U11",
+    "name": "Shinoj,Accart",
+    "phone_number": 1234667890,
+    "location": "New York",
+    "time_zone": "ZST",
+    "linkedin_url": "https://www.linkedin.com/in/Preeti Gupta/",
+    "education_ug": "BTech",
+    "education_pg": "MTech",
+    "visa_status": "Not-Specified",
+    "comments": "Tes4592759t"
+}</t>
+  </si>
+  <si>
+    <t>U156</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,217 +878,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="5" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="B5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="C5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="C6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C8" r:id="rId5"/>
-    <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="C10" r:id="rId7"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{CB2B40E9-DC7B-41B1-844B-0F78C6E0CC8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.54296875" customWidth="1"/>
+    <col min="1" max="1" width="60.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5546875" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="40.54296875" customWidth="1"/>
+    <col min="4" max="4" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1068,150 +1112,178 @@
         <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="159.5">
+    <row r="2" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="130.5">
-      <c r="A3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="159.5">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="159.5">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="159.5">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="159.5">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="159.5">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="159.5">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="159.5">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="159.5">
+    </row>
+    <row r="11" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1221,173 +1293,173 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" customWidth="1"/>
-    <col min="5" max="5" width="44.1796875" customWidth="1"/>
+    <col min="1" max="1" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="217.5">
+    <row r="2" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="217.5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="217.5">
-      <c r="A4" s="11" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="203">
-      <c r="A5" s="11" t="s">
+      <c r="B6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="203">
-      <c r="A6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="203">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="217.5">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="232">
-      <c r="A9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="D9" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1397,123 +1469,123 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="31" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="6"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>

</xml_diff>